<commit_message>
Set asset location for GitHub and email credentials as well as other email settings in config
</commit_message>
<xml_diff>
--- a/CommitTrackerPerformer/Data/Config.xlsx
+++ b/CommitTrackerPerformer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\track-commit-history\CommitTrackerPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C84056-78E8-452C-AC5B-4BB0D7D7CF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9855CF1F-CA93-4DF8-BA5F-C3071BB20EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23715" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -127,6 +127,63 @@
   </si>
   <si>
     <t>Path to directory for output files.</t>
+  </si>
+  <si>
+    <t>EmailCredentialAssetName</t>
+  </si>
+  <si>
+    <t>EmailCredentialFolderPath</t>
+  </si>
+  <si>
+    <t>EmailServer</t>
+  </si>
+  <si>
+    <t>EmailPort</t>
+  </si>
+  <si>
+    <t>OverrideEmail</t>
+  </si>
+  <si>
+    <t>Email Credentials</t>
+  </si>
+  <si>
+    <t>P3 Automation</t>
+  </si>
+  <si>
+    <t>smtp.gmail.com</t>
+  </si>
+  <si>
+    <t>wplee.327@gmail.com</t>
+  </si>
+  <si>
+    <t>Name of Orchestrator asset containing email credentials.</t>
+  </si>
+  <si>
+    <t>Path to Orchestrator folder containing email credentials.</t>
+  </si>
+  <si>
+    <t>Server for email origin.</t>
+  </si>
+  <si>
+    <t>Port for email origin.</t>
+  </si>
+  <si>
+    <t>Override email(s) that reports are sent to. Comma separated.</t>
+  </si>
+  <si>
+    <t>GitHubCredentialAssetName</t>
+  </si>
+  <si>
+    <t>GitHubCredentialFolderPath</t>
+  </si>
+  <si>
+    <t>Name of Orchestrator asset containing GitHub credentials.</t>
+  </si>
+  <si>
+    <t>Path to Orchestrator folder containing GitHub credentials.</t>
+  </si>
+  <si>
+    <t>Git Credentials</t>
   </si>
 </sst>
 </file>
@@ -502,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -569,24 +626,94 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>465</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="30">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1573,6 +1700,13 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>